<commit_message>
chore:update history jumping logic
</commit_message>
<xml_diff>
--- a/public/file/人员管理-导入人员模板.xlsx
+++ b/public/file/人员管理-导入人员模板.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\下载\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\ktzx2\smarttt-master\smarttt_foreend\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125EBAFB-6D46-4F57-B8A4-DCCBACA176DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF0290-B8CD-4D1D-8012-2A2CC0F5901D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5774" yWindow="4238" windowWidth="19562" windowHeight="8953" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +211,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -237,7 +246,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -254,6 +263,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -740,7 +752,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="12.9" x14ac:dyDescent="0.15"/>
@@ -749,7 +761,7 @@
     <col min="11" max="11" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="28.55" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -779,6 +791,9 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
@@ -814,9 +829,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.15">
-      <c r="K4" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="K4" s="5"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>

</xml_diff>